<commit_message>
Add Blok Sensus, SLS, and Desa management functionality, including routes, controllers, models, views, and migrations. Integrate PHPSpreadsheet for Excel import/export features.
</commit_message>
<xml_diff>
--- a/kode_sls.xlsx
+++ b/kode_sls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\peta-bpsenrekang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371E52AA-1C4E-4E19-BDEC-58E34F57A60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B24B9BA-895D-4B67-83E0-79700C1E4F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6029" uniqueCount="1252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6029" uniqueCount="1253">
   <si>
     <t>luas</t>
   </si>
@@ -3776,6 +3776,9 @@
   </si>
   <si>
     <t>73160400130002</t>
+  </si>
+  <si>
+    <t>73160500030004</t>
   </si>
 </sst>
 </file>
@@ -3809,13 +3812,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4128,7 +4143,7 @@
   <dimension ref="A1:L548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4189,8 +4204,8 @@
       <c r="A2">
         <v>2.9604781512530458</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
+      <c r="B2" s="1" t="s">
+        <v>1252</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -24972,6 +24987,9 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>